<commit_message>
mod: structured code for readability
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -397,9 +397,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
@@ -453,9 +453,43 @@
         <v>2025-09-18T18:10:28.783+04:00</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>2025-09-18</v>
+      </c>
+      <c r="B4" t="str">
+        <v>Pick 3</v>
+      </c>
+      <c r="C4" t="str">
+        <v>250918</v>
+      </c>
+      <c r="D4" t="str">
+        <v>8-6-1</v>
+      </c>
+      <c r="E4" t="str">
+        <v>2025-09-18T22:06:26.310+04:00</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>2025-09-18</v>
+      </c>
+      <c r="B5" t="str">
+        <v>Pick 4</v>
+      </c>
+      <c r="C5" t="str">
+        <v>250918</v>
+      </c>
+      <c r="D5" t="str">
+        <v>6-0-7-6</v>
+      </c>
+      <c r="E5" t="str">
+        <v>2025-09-18T22:06:26.310+04:00</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:E3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:E5"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>